<commit_message>
translation start, updating forms
Created a translation.xlsx sheet for entering fijian text.
Various forms updated with notes from test session.
</commit_message>
<xml_diff>
--- a/ODK-X_surveys/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/ODK-X_surveys/app/config/assets/framework/forms/framework/framework.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="179">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -471,109 +471,100 @@
     <t xml:space="preserve">Social Capital Ranking</t>
   </si>
   <si>
+    <t xml:space="preserve">branch_label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">values_list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.prompt.text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.hint.text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opendatakit.getPlatformInfo().container == "Chrome"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose a form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end if</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exit section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'?' + odkSurvey.getHashString('household_items')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">external_link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freelist: household items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'?' + odkSurvey.getHashString('household_cooperation_measures')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freelist: cooperation measures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'?' + odkSurvey.getHashString('household_census')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main household census</t>
+  </si>
+  <si>
     <t xml:space="preserve">household_member</t>
   </si>
   <si>
+    <t xml:space="preserve">'?' + odkSurvey.getHashString('household_member')</t>
+  </si>
+  <si>
     <t xml:space="preserve">.(member subform)</t>
   </si>
   <si>
-    <t xml:space="preserve">These forms are called from other forms</t>
+    <t xml:space="preserve">'?' + odkSurvey.getHashString('social_network')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social Network Questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'?' + odkSurvey.getHashString('social_capital')</t>
   </si>
   <si>
     <t xml:space="preserve">marriages</t>
   </si>
   <si>
-    <t xml:space="preserve">.(marriages subform)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">These are not to be used on their own</t>
+    <t xml:space="preserve">'?' + odkSurvey.getHashString('marriages')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.(marriage subform)</t>
   </si>
   <si>
     <t xml:space="preserve">families</t>
   </si>
   <si>
+    <t xml:space="preserve">'?' + odkSurvey.getHashString('families')</t>
+  </si>
+  <si>
     <t xml:space="preserve">.(families subform)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">branch_label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">url</t>
-  </si>
-  <si>
-    <t xml:space="preserve">condition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">values_list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display.prompt.text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display.hint.text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if</t>
-  </si>
-  <si>
-    <t xml:space="preserve">opendatakit.getPlatformInfo().container == "Chrome"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user_branch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choose a form</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end if</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exit section</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'?' + odkSurvey.getHashString('household_items')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">external_link</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Freelist: household items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'?' + odkSurvey.getHashString('household_cooperation_measures')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Freelist: cooperation measures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'?' + odkSurvey.getHashString('household_census')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Main household census</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'?' + odkSurvey.getHashString('household_member')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'?' + odkSurvey.getHashString('social_network')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social Network Questions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'?' + odkSurvey.getHashString('social_capital')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'?' + odkSurvey.getHashString('marriages')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.(marriage subform)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'?' + odkSurvey.getHashString('families')</t>
   </si>
   <si>
     <t xml:space="preserve">FROM</t>
@@ -912,11 +903,11 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="A10:D12 C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.16"/>
   </cols>
@@ -949,11 +940,11 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A10:D12 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.52"/>
@@ -1021,11 +1012,11 @@
   </sheetPr>
   <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A10:D12 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="26.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="57.83"/>
@@ -1521,11 +1512,11 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32"/>
@@ -1612,46 +1603,6 @@
         <v>143</v>
       </c>
       <c r="D8" s="5"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="D12" s="6"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -1672,11 +1623,11 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A32" activeCellId="1" sqref="A10:D12 A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.78125" defaultRowHeight="33" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="19.765625" defaultRowHeight="33" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="62.14"/>
@@ -1686,28 +1637,28 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="I1" s="8"/>
     </row>
@@ -1715,10 +1666,10 @@
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
@@ -1732,13 +1683,13 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>130</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="H3" s="9"/>
     </row>
@@ -1746,7 +1697,7 @@
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -1759,7 +1710,7 @@
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -1783,16 +1734,16 @@
     <row r="8" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="11"/>
       <c r="B8" s="12" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="H8" s="11"/>
     </row>
@@ -1800,7 +1751,7 @@
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
@@ -1823,16 +1774,16 @@
     <row r="12" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="13"/>
       <c r="B12" s="14" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="14" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="H12" s="13"/>
     </row>
@@ -1840,7 +1791,7 @@
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
@@ -1863,16 +1814,16 @@
     <row r="16" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="15"/>
       <c r="B16" s="16" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="F16" s="16"/>
       <c r="G16" s="16" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="H16" s="15"/>
     </row>
@@ -1880,7 +1831,7 @@
       <c r="A17" s="15"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
@@ -1890,7 +1841,7 @@
     </row>
     <row r="19" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -1903,16 +1854,16 @@
     <row r="20" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="11"/>
       <c r="B20" s="16" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
       <c r="E20" s="16" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="F20" s="16"/>
       <c r="G20" s="16" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="H20" s="15"/>
     </row>
@@ -1920,7 +1871,7 @@
       <c r="A21" s="11"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
@@ -1943,16 +1894,16 @@
     <row r="25" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="19"/>
       <c r="B25" s="16" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="E25" s="16" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="F25" s="16"/>
       <c r="G25" s="16" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="H25" s="20"/>
     </row>
@@ -1960,7 +1911,7 @@
       <c r="A26" s="19"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
@@ -1983,12 +1934,12 @@
     <row r="29" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="19"/>
       <c r="B29" s="16" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C29" s="16"/>
       <c r="D29" s="16"/>
       <c r="E29" s="16" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="F29" s="16"/>
       <c r="G29" s="16" t="s">
@@ -2000,7 +1951,7 @@
       <c r="A30" s="19"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
@@ -2010,7 +1961,7 @@
     </row>
     <row r="32" customFormat="false" ht="37.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="17" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
@@ -2023,16 +1974,16 @@
     <row r="33" customFormat="false" ht="37.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="19"/>
       <c r="B33" s="16" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
       <c r="E33" s="16" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="F33" s="16"/>
       <c r="G33" s="16" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="H33" s="20"/>
     </row>
@@ -2040,7 +1991,7 @@
       <c r="A34" s="19"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
@@ -2051,7 +2002,7 @@
     <row r="35" customFormat="false" ht="37.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="37.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="17" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
@@ -2064,16 +2015,16 @@
     <row r="37" customFormat="false" ht="37.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="19"/>
       <c r="B37" s="16" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
       <c r="E37" s="16" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="F37" s="16"/>
       <c r="G37" s="16" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
       <c r="H37" s="20"/>
     </row>
@@ -2081,7 +2032,7 @@
       <c r="A38" s="19"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="15"/>
@@ -2115,18 +2066,18 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="A10:D12 A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -2145,7 +2096,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
update for pilot test
</commit_message>
<xml_diff>
--- a/ODK-X_surveys/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/ODK-X_surveys/app/config/assets/framework/forms/framework/framework.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="188">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -471,6 +471,24 @@
     <t xml:space="preserve">Social Capital Ranking</t>
   </si>
   <si>
+    <t xml:space="preserve">network_member</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Network Member</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New survey network method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">individual_survey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual Survey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cooperation survey for head and spouse</t>
+  </si>
+  <si>
     <t xml:space="preserve">branch_label</t>
   </si>
   <si>
@@ -565,6 +583,43 @@
   </si>
   <si>
     <t xml:space="preserve">.(families subform)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'?' + odkSurvey.getHashString('network_member')</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'?' + odkSurvey.getHashString('</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">individual_survey</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">')</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual survey</t>
   </si>
   <si>
     <t xml:space="preserve">FROM</t>
@@ -583,7 +638,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -612,6 +667,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -739,7 +800,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -824,6 +885,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -903,11 +968,11 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="A10:D12 C15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.16"/>
   </cols>
@@ -940,11 +1005,11 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A10:D12 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.52"/>
@@ -1012,11 +1077,11 @@
   </sheetPr>
   <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A10:D12 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="26.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="57.83"/>
@@ -1512,11 +1577,11 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10:D12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32"/>
@@ -1603,6 +1668,34 @@
         <v>143</v>
       </c>
       <c r="D8" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -1623,42 +1716,42 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="1" sqref="A10:D12 A32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.765625" defaultRowHeight="33" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="19.73046875" defaultRowHeight="33" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="62.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="48.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="38.33"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="I1" s="8"/>
     </row>
@@ -1666,10 +1759,10 @@
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
@@ -1683,13 +1776,13 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>130</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="H3" s="9"/>
     </row>
@@ -1697,7 +1790,7 @@
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -1710,7 +1803,7 @@
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -1734,16 +1827,16 @@
     <row r="8" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="11"/>
       <c r="B8" s="12" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="H8" s="11"/>
     </row>
@@ -1751,7 +1844,7 @@
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
@@ -1774,16 +1867,16 @@
     <row r="12" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="13"/>
       <c r="B12" s="14" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="14" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="H12" s="13"/>
     </row>
@@ -1791,7 +1884,7 @@
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
@@ -1814,16 +1907,16 @@
     <row r="16" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="15"/>
       <c r="B16" s="16" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="F16" s="16"/>
       <c r="G16" s="16" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="H16" s="15"/>
     </row>
@@ -1831,7 +1924,7 @@
       <c r="A17" s="15"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
@@ -1841,7 +1934,7 @@
     </row>
     <row r="19" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -1854,16 +1947,16 @@
     <row r="20" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="11"/>
       <c r="B20" s="16" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
       <c r="E20" s="16" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="F20" s="16"/>
       <c r="G20" s="16" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="H20" s="15"/>
     </row>
@@ -1871,7 +1964,7 @@
       <c r="A21" s="11"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
@@ -1894,16 +1987,16 @@
     <row r="25" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="19"/>
       <c r="B25" s="16" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="E25" s="16" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="F25" s="16"/>
       <c r="G25" s="16" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="H25" s="20"/>
     </row>
@@ -1911,7 +2004,7 @@
       <c r="A26" s="19"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
@@ -1934,12 +2027,12 @@
     <row r="29" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="19"/>
       <c r="B29" s="16" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C29" s="16"/>
       <c r="D29" s="16"/>
       <c r="E29" s="16" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="F29" s="16"/>
       <c r="G29" s="16" t="s">
@@ -1951,7 +2044,7 @@
       <c r="A30" s="19"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
@@ -1961,7 +2054,7 @@
     </row>
     <row r="32" customFormat="false" ht="37.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="17" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
@@ -1974,16 +2067,16 @@
     <row r="33" customFormat="false" ht="37.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="19"/>
       <c r="B33" s="16" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
       <c r="E33" s="16" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="F33" s="16"/>
       <c r="G33" s="16" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="H33" s="20"/>
     </row>
@@ -1991,7 +2084,7 @@
       <c r="A34" s="19"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
@@ -2002,7 +2095,7 @@
     <row r="35" customFormat="false" ht="37.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="37.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="17" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
@@ -2015,16 +2108,16 @@
     <row r="37" customFormat="false" ht="37.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="19"/>
       <c r="B37" s="16" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
       <c r="E37" s="16" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="F37" s="16"/>
       <c r="G37" s="16" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="H37" s="20"/>
     </row>
@@ -2032,13 +2125,87 @@
       <c r="A38" s="19"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="15"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
       <c r="H38" s="20"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+    </row>
+    <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="11"/>
+      <c r="B41" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="11"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="11"/>
+      <c r="B45" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="F45" s="16"/>
+      <c r="G45" s="21" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="11"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
     </row>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2066,18 +2233,18 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="A10:D12 A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -2096,7 +2263,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>